<commit_message>
Update FODO sample report
</commit_message>
<xml_diff>
--- a/Archive/Report FODO-1010 Assembly Survey.xlsx
+++ b/Archive/Report FODO-1010 Assembly Survey.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" tabRatio="600" firstSheet="1" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7360" tabRatio="600" firstSheet="1" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alignment Summary" sheetId="1" state="visible" r:id="rId1"/>
@@ -533,7 +533,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -982,7 +982,7 @@
   <dimension ref="B1:H34"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1476,7 +1476,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" ht="28" customHeight="1" s="50">
+    <row r="29" ht="41" customHeight="1" s="50">
       <c r="B29" s="26" t="inlineStr">
         <is>
           <t>NOTE:</t>

</xml_diff>